<commit_message>
Updated do and slides
</commit_message>
<xml_diff>
--- a/Lab/Potential Outcomes/Potential outcomes excel.xlsx
+++ b/Lab/Potential Outcomes/Potential outcomes excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/Causal-Inference-1/Lab/Potential Outcomes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92953055-5011-DA4A-80FB-FBAD0FCA8678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ABF8C3-32D9-7246-B938-26739693080A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23720" activeTab="1" xr2:uid="{3B8309A6-345D-6346-A456-44EEA34DC221}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>Patient</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Selection bias</t>
   </si>
   <si>
-    <t>ATT (Drug)</t>
-  </si>
-  <si>
     <t>ATU (Mindfulness)</t>
   </si>
   <si>
@@ -126,151 +123,112 @@
     <t>SDO            Direct Calculation</t>
   </si>
   <si>
-    <t>Perfect doctor: treated if and only if treatment effect is 0 or positive</t>
-  </si>
-  <si>
-    <t>ATE: average treatment effect for the entire population</t>
-  </si>
-  <si>
-    <t>ATT: average treatment effect for only the people who got exercise</t>
-  </si>
-  <si>
-    <t>ATU: average treatment effect for only the people who got mindfulness</t>
-  </si>
-  <si>
-    <t>E[Y0|D=1]: average health outcome on mindfulness for those on exercise (counterfactual, but fixed and "real")</t>
-  </si>
-  <si>
-    <t>E[Y0|D=0]: average health outcome on mindfulness (state of the world) for those on mindfulness (a particular</t>
-  </si>
-  <si>
-    <t>subpopulation).  This is observed because Y=Y(0) if D=0, but Y=Y(1) if D=1, so that's why</t>
-  </si>
-  <si>
-    <t>we do not see Y(0) for D=1 (that B16 cell is technically "missing" but not B17 cell).</t>
-  </si>
-  <si>
-    <t>Selection bias: E[Y0|D=1] - E[Y0|D=0]. It just measures the differences in the two groups average Y0</t>
-  </si>
-  <si>
-    <t>pi: percent the population in the treatment</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SDO direct: Avg Y for D=1 - Avg Y for D=0.  It is simply </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>describing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> how the two groups differ on happiness</t>
-    </r>
-  </si>
-  <si>
-    <t>Switching equation: we have to assign potential outcomes to realized outcomes using treatmetn assignment</t>
-  </si>
-  <si>
-    <t>Y=DY1 + (1-D)Y0</t>
-  </si>
-  <si>
-    <t>Exercise group's realized happiness is 2.97 points lower than mindfulness group, even though</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">the ATT for that group is 4.4.  But the ATE is -1.54, so it's a </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>biased</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> estimate of the ATE.</t>
-    </r>
-  </si>
-  <si>
-    <t>as SDO direct (-2.967…)</t>
-  </si>
-  <si>
     <t>ATT (exercise)</t>
   </si>
   <si>
     <t>ATU (mindfulness)</t>
   </si>
   <si>
-    <t>The two purposes of the exercise is:</t>
-  </si>
-  <si>
-    <t>To decompose all simple comparisons into</t>
-  </si>
-  <si>
-    <t>treatment effects and bias terms</t>
-  </si>
-  <si>
-    <t>It helps us understand why randomization</t>
-  </si>
-  <si>
-    <t>will be so important; randomization will</t>
-  </si>
-  <si>
-    <t>"delete" the selection bias terms and the</t>
-  </si>
-  <si>
-    <t>"heterogenous treatment effect bias" terms.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SDO decomposition: SDO = ATE </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+ selection bias + (1-pi)*(ATT - ATU)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. It will give us the exact same number</t>
-    </r>
+    <t>Use the switching equation and assign the potential outcome to the realized outcome using the treatment assignment</t>
+  </si>
+  <si>
+    <t>"Y = 1 x 7 + (1 - 1) x 3 = 7 + 0x3 = 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">" Y = 1 x 6 + (1 - 1) x 5 = 6 </t>
+  </si>
+  <si>
+    <t>" Y = 0 x 0 + (1 - 0) x 2 = 2</t>
+  </si>
+  <si>
+    <t>" Y = 0 x 17 + (1 - 0) x 20 = 20</t>
+  </si>
+  <si>
+    <t>" Y = 0 x 5 + (1 - 0) x 14 = 14</t>
+  </si>
+  <si>
+    <t>" Y = 0 x 16 + (1 - 0) x 17 = 17</t>
+  </si>
+  <si>
+    <t>" Y = 1 x 2 + (1 - 0) x 0 = 2</t>
+  </si>
+  <si>
+    <t>" Y = 0 x 4 + (1 - 0) x 5 = 5</t>
+  </si>
+  <si>
+    <t>" Y = 0 x 14 + (1 - 0) x 15 = 15</t>
+  </si>
+  <si>
+    <t>TE     (Y1-Y0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; - The average treatment effect for Andy through Mindy is -1.54545455. That means even though Andy's treatment effect is -4, the average treatment effect is -1.54. On average exercise reduces health outcomes by 1.54 points. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is ATE?  </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>&lt; - The average treatment effect for people on exercise is called the ATT</t>
+  </si>
+  <si>
+    <t>&lt; - The average treatment effect for people on mindfulness is called the ATU</t>
+  </si>
+  <si>
+    <t>"E[ … ] means "average". It's called the "expectation operator" and in statistics, expectation just means "take the average"</t>
+  </si>
+  <si>
+    <t>ATE = E[Y1 - Y0] = E[Y1] - E[Y0] = E[TE]</t>
+  </si>
+  <si>
+    <t>ATT = E[Y1 - Y0|D=exercise] = E[Y1|D=exercise] - E[Y0|D=mindfulness]</t>
+  </si>
+  <si>
+    <t>SDO = average Y for exercise group minus average Y for mindfulness group</t>
+  </si>
+  <si>
+    <t>Avg Y for exercise group</t>
+  </si>
+  <si>
+    <t>Avg Y for mindfulness group</t>
+  </si>
+  <si>
+    <t>SDO = 9.2 - 12.17</t>
+  </si>
+  <si>
+    <t>&lt;- This number is not the ATE. The ATE was -1.54. The ATT was 4.4. The ATU was -6.5.  So this SDO is not causal. It's just a comparison between two groups' realized outcomes and it's equal to -2.967 which is not the ATE, the ATT or the ATU.</t>
+  </si>
+  <si>
+    <t>&lt; - SDO = avg Y for D=1 - avg Y for D=0</t>
+  </si>
+  <si>
+    <t>ATT (Exercise)</t>
+  </si>
+  <si>
+    <t>&lt; - Average TE</t>
+  </si>
+  <si>
+    <t>&lt; - Average TE for D=1</t>
+  </si>
+  <si>
+    <t>&lt; - Average TE for D=0</t>
+  </si>
+  <si>
+    <t>The SDO is a "biased estimate of the ATE".  Sometimes the SDO may be negative and the ATE is negative and sometimes the SDO is negative but the SDO is positive.</t>
+  </si>
+  <si>
+    <t>The SDO of people with Covid on ventilators. You'd calculate Covid symptoms for people on vents minus Covid symptoms for people not on vents (average).</t>
+  </si>
+  <si>
+    <t>It wouldn't tell you average treatmetn effect for vents; it wouldn't tell you average treatment effect for people not on vents; and it wouldn't</t>
+  </si>
+  <si>
+    <t>tell you average treatment effect for everyone.  The SDO is not measuring average treatment effects because we cannot observe individual</t>
+  </si>
+  <si>
+    <t>treatment effects. The SDO is only comparing two groups of people and treatment effects are comparing two POTENTIAL OUTCOMES for the same person.</t>
   </si>
 </sst>
 </file>
@@ -305,12 +263,10 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -387,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -522,11 +478,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -547,15 +516,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -607,15 +567,50 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -933,9 +928,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA024F43-2F9F-2140-8158-FE637C7522C5}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,27 +941,29 @@
     <col min="4" max="4" width="6.83203125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="32" t="s">
+      <c r="D1" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="F1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -975,22 +972,19 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="41">
         <v>5</v>
       </c>
       <c r="D2" s="3">
         <f>B2-C2</f>
         <v>-4</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2" s="38">
         <f>F2*B2+(1-F2)*C2</f>
         <v>5</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="26">
         <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -1000,116 +994,113 @@
       <c r="B3" s="4">
         <v>5</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="42">
         <v>15</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D12" si="0">B3-C3</f>
+        <f>B3-C3</f>
         <v>-10</v>
       </c>
-      <c r="E3" s="36">
-        <f t="shared" ref="E3:E12" si="1">F3*B3+(1-F3)*C3</f>
+      <c r="E3" s="39">
+        <f>F3*B3+(1-F3)*C3</f>
         <v>15</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="27">
         <v>0</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="42">
         <v>12</v>
       </c>
       <c r="C4" s="4">
         <v>3</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" si="0"/>
+        <f>B4-C4</f>
         <v>9</v>
       </c>
-      <c r="E4" s="36">
-        <f t="shared" si="1"/>
+      <c r="E4" s="39">
+        <f t="shared" ref="E4:E12" si="0">F4*B4+(1-F4)*C4</f>
         <v>12</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="27">
         <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="42">
         <v>19</v>
       </c>
       <c r="C5" s="4">
         <v>11</v>
       </c>
       <c r="D5" s="4">
+        <f>B5-C5</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="39">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E5" s="36">
-        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="27">
         <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="42">
         <v>7</v>
       </c>
       <c r="C6" s="4">
         <v>6</v>
       </c>
       <c r="D6" s="4">
+        <f>B6-C6</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="39">
         <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F6" s="27">
         <v>1</v>
-      </c>
-      <c r="E6" s="36">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="F6" s="30">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="42">
         <v>6</v>
       </c>
       <c r="C7" s="4">
         <v>3</v>
       </c>
       <c r="D7" s="4">
+        <f>B7-C7</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="39">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E7" s="36">
-        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="27">
         <v>1</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -1119,22 +1110,22 @@
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="42">
         <v>2</v>
       </c>
       <c r="D8" s="4">
+        <f>B8-C8</f>
+        <v>-1</v>
+      </c>
+      <c r="E8" s="39">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="E8" s="36">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="27">
         <v>0</v>
       </c>
-      <c r="I8" t="s">
-        <v>33</v>
+      <c r="G8" s="35" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -1144,22 +1135,19 @@
       <c r="B9" s="4">
         <v>19</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="42">
         <v>20</v>
       </c>
       <c r="D9" s="4">
+        <f>B9-C9</f>
+        <v>-1</v>
+      </c>
+      <c r="E9" s="39">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="E9" s="36">
-        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="27">
         <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -1169,22 +1157,19 @@
       <c r="B10" s="4">
         <v>5</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="42">
         <v>14</v>
       </c>
       <c r="D10" s="4">
+        <f>B10-C10</f>
+        <v>-9</v>
+      </c>
+      <c r="E10" s="39">
         <f t="shared" si="0"/>
-        <v>-9</v>
-      </c>
-      <c r="E10" s="36">
-        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="27">
         <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -1194,70 +1179,85 @@
       <c r="B11" s="4">
         <v>3</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="42">
         <v>17</v>
       </c>
       <c r="D11" s="4">
+        <f>B11-C11</f>
+        <v>-14</v>
+      </c>
+      <c r="E11" s="39">
         <f t="shared" si="0"/>
-        <v>-14</v>
-      </c>
-      <c r="E11" s="36">
-        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="27">
         <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="43">
         <v>2</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
       </c>
       <c r="D12" s="5">
+        <f>B12-C12</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="40">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F12" s="28">
         <v>1</v>
-      </c>
-      <c r="E12" s="37">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F12" s="31">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="44" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:16" s="2" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="I14" s="34" t="s">
-        <v>38</v>
+      <c r="C14" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="9">
+        <f xml:space="preserve"> AVERAGE(E4,E5,E6,E7,E12)</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="46"/>
+      <c r="G14" s="36">
+        <f>AVERAGE(E2,E3,E8,E9,E10,E11)</f>
+        <v>12.166666666666666</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="34">
+        <f>D14-G14</f>
+        <v>-2.9666666666666668</v>
       </c>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
@@ -1268,169 +1268,127 @@
       <c r="P14" s="34"/>
     </row>
     <row r="15" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="18">
+      <c r="A15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="15">
         <f>AVERAGE(D2:D12)</f>
         <v>-1.5454545454545454</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="25">
-        <f>AVERAGE(D4,D5,D6,D7,D12)</f>
+      <c r="A16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="22">
+        <f>AVERAGE(D4:D7,D12)</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="I16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="25">
+    </row>
+    <row r="17" spans="1:6" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="22">
         <f>AVERAGE(D2,D3,D8,D9,D10,D11)</f>
         <v>-6.5</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="I19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="20">
-        <f>AVERAGE(C4,C5,C6,C7,C12)</f>
-        <v>4.8</v>
-      </c>
+      <c r="B20" s="17"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="22">
-        <f>AVERAGE(C2,C3,C8,C9,C11,C10)</f>
-        <v>12.166666666666666</v>
-      </c>
+      <c r="B21" s="19"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="22">
-        <f>B20-B21</f>
-        <v>-7.3666666666666663</v>
-      </c>
+      <c r="B22" s="19"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="22">
-        <f>AVERAGE(F2:F12)</f>
-        <v>0.45454545454545453</v>
-      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="19"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="19">
+        <f>AVERAGE(E4,E5,E6,E7,E12)-AVERAGE(E2,E3,E8,E9,E10,E11)</f>
+        <v>-2.9666666666666668</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="22">
-        <f>AVERAGE(E4,E5,E6,E7,E12) - AVERAGE(E2,E3,E8:E11)</f>
-        <v>-2.9666666666666668</v>
-      </c>
-      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="J24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="33">
-        <f>B15+B22+(1-B23)*(B16-B17)</f>
-        <v>-2.9666666666666668</v>
-      </c>
+    </row>
+    <row r="25" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1439,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F7DDCB-91CC-874B-8191-4AC38ADF5F15}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1453,183 +1411,302 @@
     <col min="4" max="4" width="6.83203125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="41">
         <v>5</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="29"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2" s="31">
+        <f>B2-C2</f>
+        <v>-1</v>
+      </c>
+      <c r="E2" s="38">
+        <f>F2*B2+(1-F2)*C2</f>
+        <v>5</v>
+      </c>
+      <c r="F2" s="26">
+        <v>0</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4">
         <v>14</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="42">
         <v>15</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="30"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D3" s="32">
+        <f t="shared" ref="D3:D11" si="0">B3-C3</f>
+        <v>-1</v>
+      </c>
+      <c r="E3" s="39">
+        <f>F3*B3+(1-F3)*C3</f>
+        <v>15</v>
+      </c>
+      <c r="F3" s="27">
+        <v>0</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="42">
         <v>12</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="30"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4" s="32">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E4" s="39">
+        <f t="shared" ref="E4:E12" si="1">F4*B4+(1-F4)*C4</f>
+        <v>12</v>
+      </c>
+      <c r="F4" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="42">
         <v>19</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="30"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5" s="32">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E5" s="39">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="F5" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="42">
         <v>7</v>
       </c>
       <c r="C6" s="4">
         <v>3</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="30"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="32">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E6" s="39">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F6" s="27">
+        <v>1</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="42">
         <v>6</v>
       </c>
       <c r="C7" s="4">
         <v>5</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="30"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" s="32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="39">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F7" s="27">
+        <v>1</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="42">
         <v>2</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="30"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" s="32">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E8" s="39">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F8" s="27">
+        <v>0</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="4">
         <v>17</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="42">
         <v>20</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="30"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" s="32">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E9" s="39">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F9" s="27">
+        <v>0</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="4">
         <v>5</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="42">
         <v>14</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="30"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="32">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="E10" s="39">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="F10" s="27">
+        <v>0</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="4">
         <v>16</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="42">
         <v>17</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="30"/>
-    </row>
-    <row r="12" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="32">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E11" s="39">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="F11" s="27">
+        <v>0</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="43">
         <v>2</v>
       </c>
       <c r="C12" s="5">
         <v>0</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="31"/>
-    </row>
-    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="33">
+        <f>B12-C12</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="40">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F12" s="28">
+        <v>1</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1637,122 +1714,159 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="16" t="s">
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="1"/>
+      <c r="G14" s="34"/>
+    </row>
+    <row r="15" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="15">
+        <f>AVERAGE(D2:D12)</f>
+        <v>1.7272727272727273</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="1"/>
+    <row r="16" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="22">
+        <f>AVERAGE(D4,D5,D6,D7,D12)</f>
+        <v>7.2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="1"/>
+      <c r="H16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="22">
+        <f>AVERAGE(D2,D3,D8,D9,D10,D11)</f>
+        <v>-2.8333333333333335</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="I18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="I19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="20"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+    <row r="21" spans="1:9" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="22"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="G21" s="34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="22"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="22"/>
+    <row r="23" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="19"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="1"/>
+    <row r="24" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="19">
+        <f>AVERAGE(E4,E5,E6,E7,E12) - AVERAGE(E2,E3,E8,E9,E10,E11)</f>
+        <v>-2.9666666666666668</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="33"/>
+    <row r="25" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>